<commit_message>
GA results. Varied spacing and phase. Amplitude static.
</commit_message>
<xml_diff>
--- a/matlab/experiment/28Aug/30deg/sim30deg1.xlsx
+++ b/matlab/experiment/28Aug/30deg/sim30deg1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltd\OneDrive\Documents\2021\semester2\thesis-2021\matlab\experiment\28Aug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltd\OneDrive\Documents\2021\semester2\thesis-2021\matlab\experiment\28Aug\30deg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D37A0E-6C39-4081-82A7-6F76287F1976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6EECE0-7168-44ED-BEC8-8AE5431D6E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9744" yWindow="3480" windowWidth="19812" windowHeight="11616" xr2:uid="{4CC82A57-8492-4D0C-BA7E-13969CC221A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4CC82A57-8492-4D0C-BA7E-13969CC221A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3479,16 +3479,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3518,15 +3518,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3551,6 +3551,106 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>174313</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4DD58FE-D490-4C5E-9B5C-72BFF4AA81E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="83820"/>
+          <a:ext cx="7489513" cy="3863340"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>121165</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>124785</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FA51C7A-F5D9-4E38-A268-6EC295FA3C3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7436365" y="0"/>
+          <a:ext cx="5289035" cy="3965265"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3853,85 +3953,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F88FF0-1C6A-41A6-B982-8E90DB47F43B}">
-  <dimension ref="B15:H18"/>
+  <dimension ref="B23:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
         <v>5</v>
       </c>
-      <c r="C15">
+      <c r="C23">
         <v>0.49199999999999999</v>
       </c>
-      <c r="D15">
+      <c r="D23">
         <v>0.57699999999999996</v>
       </c>
-      <c r="E15">
+      <c r="E23">
         <v>0.47199999999999998</v>
       </c>
-      <c r="F15">
+      <c r="F23">
         <v>0.57699999999999996</v>
       </c>
-      <c r="G15">
+      <c r="G23">
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>6</v>
       </c>
-      <c r="C16">
+      <c r="C24">
         <v>245</v>
       </c>
-      <c r="D16">
+      <c r="D24">
         <v>136.30000000000001</v>
       </c>
-      <c r="E16">
+      <c r="E24">
         <v>53.8</v>
       </c>
-      <c r="F16">
+      <c r="F24">
         <v>311.5</v>
       </c>
-      <c r="G16">
+      <c r="G24">
         <v>210.3</v>
       </c>
-      <c r="H16">
+      <c r="H24">
         <v>123.9</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
         <v>7</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>8</v>
       </c>
-      <c r="C18">
+      <c r="C26">
         <v>-4.369869142886496</v>
       </c>
     </row>

</xml_diff>